<commit_message>
Update login, sign-up view and add profile pic view, and Roboto font
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/napatswift/courses/software-contruct/project-641-mercury/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95203987-D1BD-EF4A-AAE6-3B467E97C0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B40F07-07C8-D84B-9F4E-AC7F724222C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="16460" xr2:uid="{749677C9-B7DD-CA46-961A-5738EE09DB78}"/>
+    <workbookView xWindow="760" yWindow="9880" windowWidth="28040" windowHeight="16460" xr2:uid="{749677C9-B7DD-CA46-961A-5738EE09DB78}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>user_id</t>
   </si>
@@ -67,15 +67,6 @@
     <t>napatswift</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>napat</t>
-  </si>
-  <si>
-    <t>dollapavijit</t>
-  </si>
-  <si>
     <t>NAPAT1</t>
   </si>
   <si>
@@ -101,6 +92,27 @@
   </si>
   <si>
     <t>store's name, if user</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>Napat</t>
+  </si>
+  <si>
+    <t>picturePath</t>
+  </si>
+  <si>
+    <t>isBanned</t>
+  </si>
+  <si>
+    <t>loginAttempt</t>
+  </si>
+  <si>
+    <t>hasStore</t>
+  </si>
+  <si>
+    <t>store</t>
   </si>
 </sst>
 </file>
@@ -452,15 +464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DF719C-D506-6249-9E53-36E8121791ED}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,28 +480,34 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -497,16 +515,19 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -532,7 +553,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,7 +561,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,7 +585,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -572,7 +593,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,7 +601,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -588,7 +609,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -596,7 +617,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>